<commit_message>
Ajout du tir des ennemis basiques et du regard du jeu sur le tir des autres ennemis.
</commit_message>
<xml_diff>
--- a/Log de tâche.xlsx
+++ b/Log de tâche.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
   <si>
     <t>Date</t>
   </si>
@@ -120,6 +120,12 @@
   </si>
   <si>
     <t>Il y avait beaucoup de memory leaks, que j'ai fixés dans toute leur intégralité. Je vais fusionner avec la version de mon partenaire et voir s'il y a de nouveaux memory leaks.</t>
+  </si>
+  <si>
+    <t>Ajouts de contenu dans la classe des bonus. Fixatif de la classe stack. Liaison du score au HUD, mise en place des collisions des bonus. Correctif des Sujets et des Observateurs, recherche de sprites pour les Bonus et les Vaisseaux. Organisation de certaines classes, suppression de méthodes inutiles, clean-up de la mémoire (destructeurs) et codification des tests unitaires de la classe stack.</t>
+  </si>
+  <si>
+    <t>Le mariage du vecteur et de la stack a montré quelques mauvaises suprises qui ont été corrigées et détectée grace aux tests unitaires. J'ai aussi utilisé par accident getlocalbounds au lieu de getglobalbounds pour les collisions, ce fut déplaisant.</t>
   </si>
 </sst>
 </file>
@@ -883,8 +889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1015,11 +1021,19 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
+    <row r="10" spans="1:4" ht="225" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>43071</v>
+      </c>
+      <c r="B10" s="4">
+        <v>8</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>

</xml_diff>